<commit_message>
Fixed controller issue which was faulting on postback with partial view
</commit_message>
<xml_diff>
--- a/Dev Notes/Backlogs/Master Backlog.xlsx
+++ b/Dev Notes/Backlogs/Master Backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -411,7 +411,7 @@
     <t>Honda Accord Jack - Salvage Yards - 630-860-2000</t>
   </si>
   <si>
-    <t>Carey's Reference</t>
+    <t>BACKLOG</t>
   </si>
 </sst>
 </file>
@@ -867,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -919,124 +919,116 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="10" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="27" t="s">
-        <v>113</v>
+      <c r="A10" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="27" t="s">
+      <c r="A11" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="10" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="B16" s="24" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>0</v>
+      <c r="A17" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18" s="22" t="s">
+      <c r="A18" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="18" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>102</v>
+    <row r="22" spans="1:2">
+      <c r="A22" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
-        <v>29</v>
+      <c r="A23" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="18" t="s">
+      <c r="A24" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B24" s="23" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bunch of Notes changes.
</commit_message>
<xml_diff>
--- a/Dev Notes/Backlogs/Master Backlog.xlsx
+++ b/Dev Notes/Backlogs/Master Backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="135">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -348,9 +348,6 @@
     <t>Goto the Doctor and get checked up</t>
   </si>
   <si>
-    <t>Sell the Honda</t>
-  </si>
-  <si>
     <t>New Honda Problem List</t>
   </si>
   <si>
@@ -360,15 +357,9 @@
     <t>De-commission / replace Big Blue / Get a Monitor</t>
   </si>
   <si>
-    <t>Get Bins, Clean Garage</t>
-  </si>
-  <si>
     <t>Continue to Review WCF Page 91 thur 208</t>
   </si>
   <si>
-    <t>JQuery + Crockford</t>
-  </si>
-  <si>
     <t>Read the ACIM Text</t>
   </si>
   <si>
@@ -408,10 +399,34 @@
     <t>Configure Automatic Backups</t>
   </si>
   <si>
-    <t>Honda Accord Jack - Salvage Yards - 630-860-2000</t>
-  </si>
-  <si>
     <t>BACKLOG</t>
+  </si>
+  <si>
+    <t>Aleks and Maria Bills</t>
+  </si>
+  <si>
+    <t>Get some Moby from somewhere online</t>
+  </si>
+  <si>
+    <t>TO DO</t>
+  </si>
+  <si>
+    <t>ON HOLD, MANE!</t>
+  </si>
+  <si>
+    <t>Aleks Do Taxes - find CPA</t>
+  </si>
+  <si>
+    <t>WAITING TO CALL</t>
+  </si>
+  <si>
+    <t>SUNDAY EVENING</t>
+  </si>
+  <si>
+    <t>JQuery, then back to Pleiades</t>
+  </si>
+  <si>
+    <t>Honda Accord Jack - Salvage Yards - 630-860-2000 =&gt; go get it!</t>
   </si>
 </sst>
 </file>
@@ -558,9 +573,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -572,6 +584,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -867,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -897,7 +910,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>0</v>
@@ -905,7 +918,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>0</v>
@@ -919,7 +932,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="10" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>0</v>
@@ -927,33 +940,33 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="26" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="25" t="s">
-        <v>113</v>
+      <c r="A11" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>102</v>
       </c>
     </row>
@@ -965,33 +978,33 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>0</v>
+        <v>126</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" s="23" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>102</v>
       </c>
     </row>
@@ -999,15 +1012,15 @@
       <c r="A19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="25" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1018,17 +1031,25 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="18" t="s">
+      <c r="B24" s="27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1053,42 +1074,42 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1118,7 +1139,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>27</v>
@@ -1153,7 +1174,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>